<commit_message>
excel spreadsheets for data analysis
</commit_message>
<xml_diff>
--- a/data/healthy_cluster_analysis.xlsx
+++ b/data/healthy_cluster_analysis.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="statistics p(x) ~ D(x)^2" sheetId="1" r:id="rId1"/>
     <sheet name="statistics p(x) ~ 1-e^(-D(x)^2)" sheetId="3" r:id="rId2"/>
     <sheet name="error analysis" sheetId="2" r:id="rId3"/>
     <sheet name="variance over alpha" sheetId="4" r:id="rId4"/>
+    <sheet name="comparison" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="36">
   <si>
     <t>m4</t>
   </si>
@@ -129,6 +130,12 @@
   </si>
   <si>
     <t>normalized</t>
+  </si>
+  <si>
+    <t>exponential</t>
+  </si>
+  <si>
+    <t>quadratic</t>
   </si>
 </sst>
 </file>
@@ -705,7 +712,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -924,7 +930,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1044,7 +1049,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1199,7 +1203,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1427,7 +1430,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1552,7 +1554,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1707,7 +1708,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1944,7 +1944,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2068,7 +2067,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2223,7 +2221,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2458,7 +2455,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2579,7 +2575,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2654,7 +2649,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2766,7 +2760,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2934,7 +2927,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3055,7 +3047,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3128,6 +3119,716 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>10-Cluster</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Voxel Distribution</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1-e^(-a*D(x)^2)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>comparison!$O$6:$X$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>1.0708355679911786E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.5748085947781147E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.5697634367825935E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.5972639346153658E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6301288399625288E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.567666496630208E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.5469490022814553E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.5081040356457144E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.5367534367918621E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.4861646499759776E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>comparison!$O$6:$X$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>1.0708355679911786E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.5748085947781147E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.5697634367825935E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.5972639346153658E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6301288399625288E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.567666496630208E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.5469490022814553E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.5081040356457144E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.5367534367918621E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.4861646499759776E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>comparison!$D$6:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.107431917119427</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8280295616373595E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.100457260486619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10121351196301399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10290486957108599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7918536766442799E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8513144129855207E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8515506361151403E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.8029561637363705E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.6735396348665306E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DAB-4CD9-A337-371278F2A2A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>D(x)^2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>comparison!$O$7:$X$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>4.5796095612266774E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.6255655285125194E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.4111565300479876E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.740509527486745E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.6672686712526848E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.7898415877005163E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.1545908608135134E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.6746774164383685E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.8337471750706615E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.1826579369596157E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>comparison!$O$7:$X$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>4.5796095612266774E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.6255655285125194E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.4111565300479876E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.740509527486745E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.6672686712526848E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.7898415877005163E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.1545908608135134E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.6746774164383685E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.8337471750706615E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.1826579369596157E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>comparison!$D$7:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.7890527452502304E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7156548442614593E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.101311038369385</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8734856410083296E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.78959268383221E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.100953666520433</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.96969594708602E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10334660682347301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.100832180339486</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.102181689332838</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1DAB-4CD9-A337-371278F2A2A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="278760168"/>
+        <c:axId val="278760496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="278760168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cluster</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> #</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="278760496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="278760496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Voxels</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="278760168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5665,7 +6366,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5857,7 +6557,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5977,7 +6676,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6132,7 +6830,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6333,7 +7030,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6458,7 +7154,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6613,7 +7308,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6823,7 +7517,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6943,7 +7636,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7254,6 +7946,46 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10129,6 +10861,509 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15031,12 +16266,12 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>207169</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>107156</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>245269</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>135731</xdr:rowOff>
     </xdr:to>
@@ -15064,20 +16299,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>130968</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>138113</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>159543</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>176213</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>64293</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>268741</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>6123</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>316366</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>177573</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -15360,8 +16630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y120"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99"/>
+    <sheetView topLeftCell="A92" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120:M120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16397,8 +17667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17534,8 +18804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17931,4 +19201,153 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:X7"/>
+  <sheetViews>
+    <sheetView topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:X7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>0.107431917119427</v>
+      </c>
+      <c r="E6">
+        <v>9.8280295616373595E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.100457260486619</v>
+      </c>
+      <c r="G6">
+        <v>0.10121351196301399</v>
+      </c>
+      <c r="H6">
+        <v>0.10290486957108599</v>
+      </c>
+      <c r="I6">
+        <v>9.7918536766442799E-2</v>
+      </c>
+      <c r="J6">
+        <v>9.8513144129855207E-2</v>
+      </c>
+      <c r="K6">
+        <v>9.8515506361151403E-2</v>
+      </c>
+      <c r="L6">
+        <v>9.8029561637363705E-2</v>
+      </c>
+      <c r="M6">
+        <v>9.6735396348665306E-2</v>
+      </c>
+      <c r="O6">
+        <v>1.0708355679911786E-2</v>
+      </c>
+      <c r="P6">
+        <v>1.5748085947781147E-2</v>
+      </c>
+      <c r="Q6">
+        <v>1.5697634367825935E-2</v>
+      </c>
+      <c r="R6">
+        <v>1.5972639346153658E-2</v>
+      </c>
+      <c r="S6">
+        <v>1.6301288399625288E-2</v>
+      </c>
+      <c r="T6">
+        <v>1.567666496630208E-2</v>
+      </c>
+      <c r="U6">
+        <v>1.5469490022814553E-2</v>
+      </c>
+      <c r="V6">
+        <v>1.5081040356457144E-2</v>
+      </c>
+      <c r="W6">
+        <v>1.5367534367918621E-2</v>
+      </c>
+      <c r="X6">
+        <v>1.4861646499759776E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>9.7890527452502304E-2</v>
+      </c>
+      <c r="E7">
+        <v>9.7156548442614593E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.101311038369385</v>
+      </c>
+      <c r="G7">
+        <v>9.8734856410083296E-2</v>
+      </c>
+      <c r="H7">
+        <v>9.78959268383221E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.100953666520433</v>
+      </c>
+      <c r="J7">
+        <v>9.96969594708602E-2</v>
+      </c>
+      <c r="K7">
+        <v>0.10334660682347301</v>
+      </c>
+      <c r="L7">
+        <v>0.100832180339486</v>
+      </c>
+      <c r="M7">
+        <v>0.102181689332838</v>
+      </c>
+      <c r="O7">
+        <v>4.5796095612266774E-2</v>
+      </c>
+      <c r="P7">
+        <v>4.6255655285125194E-2</v>
+      </c>
+      <c r="Q7">
+        <v>4.4111565300479876E-2</v>
+      </c>
+      <c r="R7">
+        <v>4.740509527486745E-2</v>
+      </c>
+      <c r="S7">
+        <v>4.6672686712526848E-2</v>
+      </c>
+      <c r="T7">
+        <v>4.7898415877005163E-2</v>
+      </c>
+      <c r="U7">
+        <v>5.1545908608135134E-2</v>
+      </c>
+      <c r="V7">
+        <v>4.6746774164383685E-2</v>
+      </c>
+      <c r="W7">
+        <v>4.8337471750706615E-2</v>
+      </c>
+      <c r="X7">
+        <v>5.1826579369596157E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>